<commit_message>
Actulizado orden de ruta
</commit_message>
<xml_diff>
--- a/sofiback/public/preparacion.xlsx
+++ b/sofiback/public/preparacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sofi\sofiback\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\sofi\sofiback\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B9AFFB-2103-4317-8834-B00DBEA33114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C2DA1D-C6DF-46B5-90A6-8830328F9540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF0A4972-0071-4689-8DFE-231579572FAE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF0A4972-0071-4689-8DFE-231579572FAE}"/>
   </bookViews>
   <sheets>
     <sheet name="hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="A">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">hoja1!$A$1:$AD$96</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -155,7 +155,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,20 +180,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBE4D5"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -301,71 +289,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF4472C4"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF4472C4"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF4472C4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB4C6E7"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF4472C4"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF4472C4"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB4C6E7"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB4C6E7"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF4472C4"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF4472C4"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB4C6E7"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB4C6E7"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF4472C4"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF4472C4"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB4C6E7"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB4C6E7"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -397,28 +325,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -427,6 +333,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -745,87 +657,87 @@
   <dimension ref="A1:AE140"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="56" zoomScaleSheetLayoutView="70" zoomScalePageLayoutView="47" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="58.85546875" style="7" customWidth="1"/>
-    <col min="7" max="30" width="14.85546875" style="2" customWidth="1"/>
-    <col min="32" max="35" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" style="7" customWidth="1"/>
+    <col min="7" max="30" width="14.88671875" style="2" customWidth="1"/>
+    <col min="32" max="35" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="49.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:31" ht="49.95" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="31">
+      <c r="G1" s="20">
         <f ca="1">TODAY()</f>
-        <v>45877</v>
+        <v>45906</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:31" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="32" t="s">
+    <row r="2" spans="1:31" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
       <c r="AB2"/>
       <c r="AC2"/>
       <c r="AD2"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
       <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
@@ -902,7 +814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
@@ -935,13 +847,13 @@
       <c r="AD4" s="16"/>
       <c r="AE4" s="6"/>
     </row>
-    <row r="5" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="17"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="13"/>
       <c r="H5" s="14"/>
       <c r="I5" s="15"/>
@@ -966,14 +878,15 @@
       <c r="AB5" s="14"/>
       <c r="AC5" s="15"/>
       <c r="AD5" s="16"/>
-    </row>
-    <row r="6" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="18"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="19"/>
+      <c r="AE5" s="6"/>
+    </row>
+    <row r="6" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="13"/>
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
@@ -998,14 +911,15 @@
       <c r="AB6" s="14"/>
       <c r="AC6" s="15"/>
       <c r="AD6" s="16"/>
-    </row>
-    <row r="7" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE6" s="6"/>
+    </row>
+    <row r="7" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
       <c r="D7" s="10"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="17"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="13"/>
       <c r="H7" s="14"/>
       <c r="I7" s="15"/>
@@ -1030,14 +944,14 @@
       <c r="AB7" s="14"/>
       <c r="AC7" s="15"/>
       <c r="AD7" s="16"/>
-      <c r="AE7"/>
-    </row>
-    <row r="8" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
+      <c r="AE7" s="6"/>
+    </row>
+    <row r="8" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="12"/>
       <c r="G8" s="13"/>
       <c r="H8" s="14"/>
@@ -1063,14 +977,15 @@
       <c r="AB8" s="14"/>
       <c r="AC8" s="15"/>
       <c r="AD8" s="16"/>
-    </row>
-    <row r="9" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE8" s="6"/>
+    </row>
+    <row r="9" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
       <c r="D9" s="10"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="17"/>
+      <c r="F9" s="12"/>
       <c r="G9" s="13"/>
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
@@ -1095,14 +1010,15 @@
       <c r="AB9" s="14"/>
       <c r="AC9" s="15"/>
       <c r="AD9" s="16"/>
-    </row>
-    <row r="10" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19"/>
+      <c r="AE9" s="6"/>
+    </row>
+    <row r="10" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
       <c r="G10" s="13"/>
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
@@ -1127,13 +1043,14 @@
       <c r="AB10" s="14"/>
       <c r="AC10" s="15"/>
       <c r="AD10" s="16"/>
-    </row>
-    <row r="11" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="24"/>
+      <c r="AE10" s="6"/>
+    </row>
+    <row r="11" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
       <c r="H11" s="14"/>
@@ -1159,14 +1076,15 @@
       <c r="AB11" s="14"/>
       <c r="AC11" s="15"/>
       <c r="AD11" s="16"/>
-    </row>
-    <row r="12" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE11" s="6"/>
+    </row>
+    <row r="12" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="17"/>
+      <c r="F12" s="12"/>
       <c r="G12" s="13"/>
       <c r="H12" s="14"/>
       <c r="I12" s="15"/>
@@ -1191,14 +1109,15 @@
       <c r="AB12" s="14"/>
       <c r="AC12" s="15"/>
       <c r="AD12" s="16"/>
-    </row>
-    <row r="13" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="22"/>
+      <c r="AE12" s="6"/>
+    </row>
+    <row r="13" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
       <c r="I13" s="15"/>
@@ -1223,14 +1142,15 @@
       <c r="AB13" s="14"/>
       <c r="AC13" s="15"/>
       <c r="AD13" s="16"/>
-    </row>
-    <row r="14" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE13" s="6"/>
+    </row>
+    <row r="14" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
       <c r="D14" s="10"/>
       <c r="E14" s="11"/>
-      <c r="F14" s="17"/>
+      <c r="F14" s="12"/>
       <c r="G14" s="13"/>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
@@ -1255,14 +1175,15 @@
       <c r="AB14" s="14"/>
       <c r="AC14" s="15"/>
       <c r="AD14" s="16"/>
-    </row>
-    <row r="15" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="19"/>
+      <c r="AE14" s="6"/>
+    </row>
+    <row r="15" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
       <c r="G15" s="13"/>
       <c r="H15" s="14"/>
       <c r="I15" s="15"/>
@@ -1287,14 +1208,15 @@
       <c r="AB15" s="14"/>
       <c r="AC15" s="15"/>
       <c r="AD15" s="16"/>
-    </row>
-    <row r="16" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE15" s="6"/>
+    </row>
+    <row r="16" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
-      <c r="F16" s="17"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="13"/>
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
@@ -1319,14 +1241,14 @@
       <c r="AB16" s="14"/>
       <c r="AC16" s="15"/>
       <c r="AD16" s="16"/>
-      <c r="AE16"/>
-    </row>
-    <row r="17" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
+      <c r="AE16" s="6"/>
+    </row>
+    <row r="17" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="12"/>
       <c r="G17" s="13"/>
       <c r="H17" s="14"/>
@@ -1352,14 +1274,15 @@
       <c r="AB17" s="14"/>
       <c r="AC17" s="15"/>
       <c r="AD17" s="16"/>
-    </row>
-    <row r="18" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE17" s="6"/>
+    </row>
+    <row r="18" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
       <c r="D18" s="10"/>
       <c r="E18" s="11"/>
-      <c r="F18" s="17"/>
+      <c r="F18" s="12"/>
       <c r="G18" s="13"/>
       <c r="H18" s="14"/>
       <c r="I18" s="15"/>
@@ -1384,14 +1307,15 @@
       <c r="AB18" s="14"/>
       <c r="AC18" s="15"/>
       <c r="AD18" s="16"/>
-    </row>
-    <row r="19" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="19"/>
+      <c r="AE18" s="6"/>
+    </row>
+    <row r="19" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
       <c r="G19" s="13"/>
       <c r="H19" s="14"/>
       <c r="I19" s="15"/>
@@ -1416,13 +1340,14 @@
       <c r="AB19" s="14"/>
       <c r="AC19" s="15"/>
       <c r="AD19" s="16"/>
-    </row>
-    <row r="20" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="24"/>
+      <c r="AE19" s="6"/>
+    </row>
+    <row r="20" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="12"/>
       <c r="G20" s="13"/>
       <c r="H20" s="14"/>
@@ -1448,14 +1373,15 @@
       <c r="AB20" s="14"/>
       <c r="AC20" s="15"/>
       <c r="AD20" s="16"/>
-    </row>
-    <row r="21" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE20" s="6"/>
+    </row>
+    <row r="21" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="11"/>
-      <c r="F21" s="17"/>
+      <c r="F21" s="12"/>
       <c r="G21" s="13"/>
       <c r="H21" s="14"/>
       <c r="I21" s="15"/>
@@ -1480,14 +1406,15 @@
       <c r="AB21" s="14"/>
       <c r="AC21" s="15"/>
       <c r="AD21" s="16"/>
-    </row>
-    <row r="22" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="22"/>
+      <c r="AE21" s="6"/>
+    </row>
+    <row r="22" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="13"/>
       <c r="H22" s="14"/>
       <c r="I22" s="15"/>
@@ -1512,14 +1439,15 @@
       <c r="AB22" s="14"/>
       <c r="AC22" s="15"/>
       <c r="AD22" s="16"/>
-    </row>
-    <row r="23" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE22" s="6"/>
+    </row>
+    <row r="23" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
       <c r="D23" s="10"/>
       <c r="E23" s="11"/>
-      <c r="F23" s="17"/>
+      <c r="F23" s="12"/>
       <c r="G23" s="13"/>
       <c r="H23" s="14"/>
       <c r="I23" s="15"/>
@@ -1544,14 +1472,15 @@
       <c r="AB23" s="14"/>
       <c r="AC23" s="15"/>
       <c r="AD23" s="16"/>
-    </row>
-    <row r="24" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="19"/>
+      <c r="AE23" s="6"/>
+    </row>
+    <row r="24" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
       <c r="G24" s="13"/>
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
@@ -1576,14 +1505,15 @@
       <c r="AB24" s="14"/>
       <c r="AC24" s="15"/>
       <c r="AD24" s="16"/>
-    </row>
-    <row r="25" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE24" s="6"/>
+    </row>
+    <row r="25" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="11"/>
-      <c r="F25" s="17"/>
+      <c r="F25" s="12"/>
       <c r="G25" s="13"/>
       <c r="H25" s="14"/>
       <c r="I25" s="15"/>
@@ -1608,14 +1538,14 @@
       <c r="AB25" s="14"/>
       <c r="AC25" s="15"/>
       <c r="AD25" s="16"/>
-      <c r="AE25"/>
-    </row>
-    <row r="26" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
+      <c r="AE25" s="6"/>
+    </row>
+    <row r="26" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="12"/>
       <c r="G26" s="13"/>
       <c r="H26" s="14"/>
@@ -1641,14 +1571,15 @@
       <c r="AB26" s="14"/>
       <c r="AC26" s="15"/>
       <c r="AD26" s="16"/>
-    </row>
-    <row r="27" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE26" s="6"/>
+    </row>
+    <row r="27" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
       <c r="D27" s="10"/>
       <c r="E27" s="11"/>
-      <c r="F27" s="17"/>
+      <c r="F27" s="12"/>
       <c r="G27" s="13"/>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
@@ -1673,14 +1604,15 @@
       <c r="AB27" s="14"/>
       <c r="AC27" s="15"/>
       <c r="AD27" s="16"/>
-    </row>
-    <row r="28" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="19"/>
+      <c r="AE27" s="6"/>
+    </row>
+    <row r="28" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="12"/>
       <c r="G28" s="13"/>
       <c r="H28" s="14"/>
       <c r="I28" s="15"/>
@@ -1705,13 +1637,14 @@
       <c r="AB28" s="14"/>
       <c r="AC28" s="15"/>
       <c r="AD28" s="16"/>
-    </row>
-    <row r="29" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="24"/>
+      <c r="AE28" s="6"/>
+    </row>
+    <row r="29" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="12"/>
       <c r="G29" s="13"/>
       <c r="H29" s="14"/>
@@ -1737,14 +1670,15 @@
       <c r="AB29" s="14"/>
       <c r="AC29" s="15"/>
       <c r="AD29" s="16"/>
-    </row>
-    <row r="30" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE29" s="6"/>
+    </row>
+    <row r="30" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="9"/>
       <c r="D30" s="10"/>
       <c r="E30" s="11"/>
-      <c r="F30" s="17"/>
+      <c r="F30" s="12"/>
       <c r="G30" s="13"/>
       <c r="H30" s="14"/>
       <c r="I30" s="15"/>
@@ -1769,14 +1703,15 @@
       <c r="AB30" s="14"/>
       <c r="AC30" s="15"/>
       <c r="AD30" s="16"/>
-    </row>
-    <row r="31" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="22"/>
+      <c r="AE30" s="6"/>
+    </row>
+    <row r="31" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="12"/>
       <c r="G31" s="13"/>
       <c r="H31" s="14"/>
       <c r="I31" s="15"/>
@@ -1801,14 +1736,15 @@
       <c r="AB31" s="14"/>
       <c r="AC31" s="15"/>
       <c r="AD31" s="16"/>
-    </row>
-    <row r="32" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="19"/>
+      <c r="AE31" s="6"/>
+    </row>
+    <row r="32" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="12"/>
       <c r="G32" s="13"/>
       <c r="H32" s="14"/>
       <c r="I32" s="15"/>
@@ -1833,14 +1769,15 @@
       <c r="AB32" s="14"/>
       <c r="AC32" s="15"/>
       <c r="AD32" s="16"/>
-    </row>
-    <row r="33" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="22"/>
+      <c r="AE32" s="6"/>
+    </row>
+    <row r="33" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="12"/>
       <c r="G33" s="13"/>
       <c r="H33" s="14"/>
       <c r="I33" s="15"/>
@@ -1865,14 +1802,15 @@
       <c r="AB33" s="14"/>
       <c r="AC33" s="15"/>
       <c r="AD33" s="16"/>
-    </row>
-    <row r="34" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="19"/>
+      <c r="AE33" s="6"/>
+    </row>
+    <row r="34" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="12"/>
       <c r="G34" s="13"/>
       <c r="H34" s="14"/>
       <c r="I34" s="15"/>
@@ -1897,14 +1835,15 @@
       <c r="AB34" s="14"/>
       <c r="AC34" s="15"/>
       <c r="AD34" s="16"/>
-    </row>
-    <row r="35" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="22"/>
+      <c r="AE34" s="6"/>
+    </row>
+    <row r="35" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="12"/>
       <c r="G35" s="13"/>
       <c r="H35" s="14"/>
       <c r="I35" s="15"/>
@@ -1929,15 +1868,15 @@
       <c r="AB35" s="14"/>
       <c r="AC35" s="15"/>
       <c r="AD35" s="16"/>
-      <c r="AE35"/>
-    </row>
-    <row r="36" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="19"/>
+      <c r="AE35" s="6"/>
+    </row>
+    <row r="36" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="12"/>
       <c r="G36" s="13"/>
       <c r="H36" s="14"/>
       <c r="I36" s="15"/>
@@ -1962,15 +1901,15 @@
       <c r="AB36" s="14"/>
       <c r="AC36" s="15"/>
       <c r="AD36" s="16"/>
-      <c r="AE36"/>
-    </row>
-    <row r="37" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A37" s="21"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="22"/>
+      <c r="AE36" s="6"/>
+    </row>
+    <row r="37" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="12"/>
       <c r="G37" s="13"/>
       <c r="H37" s="14"/>
       <c r="I37" s="15"/>
@@ -1995,15 +1934,15 @@
       <c r="AB37" s="14"/>
       <c r="AC37" s="15"/>
       <c r="AD37" s="16"/>
-      <c r="AE37"/>
-    </row>
-    <row r="38" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="19"/>
+      <c r="AE37" s="6"/>
+    </row>
+    <row r="38" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
       <c r="G38" s="13"/>
       <c r="H38" s="14"/>
       <c r="I38" s="15"/>
@@ -2028,15 +1967,15 @@
       <c r="AB38" s="14"/>
       <c r="AC38" s="15"/>
       <c r="AD38" s="16"/>
-      <c r="AE38"/>
-    </row>
-    <row r="39" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="22"/>
+      <c r="AE38" s="6"/>
+    </row>
+    <row r="39" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="12"/>
       <c r="G39" s="13"/>
       <c r="H39" s="14"/>
       <c r="I39" s="15"/>
@@ -2061,15 +2000,15 @@
       <c r="AB39" s="14"/>
       <c r="AC39" s="15"/>
       <c r="AD39" s="16"/>
-      <c r="AE39"/>
-    </row>
-    <row r="40" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="22"/>
+      <c r="AE39" s="6"/>
+    </row>
+    <row r="40" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="12"/>
       <c r="G40" s="13"/>
       <c r="H40" s="14"/>
       <c r="I40" s="15"/>
@@ -2094,15 +2033,15 @@
       <c r="AB40" s="14"/>
       <c r="AC40" s="15"/>
       <c r="AD40" s="16"/>
-      <c r="AE40"/>
-    </row>
-    <row r="41" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="19"/>
+      <c r="AE40" s="6"/>
+    </row>
+    <row r="41" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="12"/>
       <c r="G41" s="13"/>
       <c r="H41" s="14"/>
       <c r="I41" s="15"/>
@@ -2127,15 +2066,15 @@
       <c r="AB41" s="14"/>
       <c r="AC41" s="15"/>
       <c r="AD41" s="16"/>
-      <c r="AE41"/>
-    </row>
-    <row r="42" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="26"/>
+      <c r="AE41" s="6"/>
+    </row>
+    <row r="42" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="12"/>
       <c r="G42" s="13"/>
       <c r="H42" s="14"/>
       <c r="I42" s="15"/>
@@ -2160,15 +2099,15 @@
       <c r="AB42" s="14"/>
       <c r="AC42" s="15"/>
       <c r="AD42" s="16"/>
-      <c r="AE42"/>
-    </row>
-    <row r="43" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="26"/>
+      <c r="AE42" s="6"/>
+    </row>
+    <row r="43" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="12"/>
       <c r="G43" s="13"/>
       <c r="H43" s="14"/>
       <c r="I43" s="15"/>
@@ -2193,15 +2132,15 @@
       <c r="AB43" s="14"/>
       <c r="AC43" s="15"/>
       <c r="AD43" s="16"/>
-      <c r="AE43"/>
-    </row>
-    <row r="44" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="26"/>
+      <c r="AE43" s="6"/>
+    </row>
+    <row r="44" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="12"/>
       <c r="G44" s="13"/>
       <c r="H44" s="14"/>
       <c r="I44" s="15"/>
@@ -2226,15 +2165,15 @@
       <c r="AB44" s="14"/>
       <c r="AC44" s="15"/>
       <c r="AD44" s="16"/>
-      <c r="AE44"/>
-    </row>
-    <row r="45" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="26"/>
+      <c r="AE44" s="6"/>
+    </row>
+    <row r="45" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="12"/>
       <c r="G45" s="13"/>
       <c r="H45" s="14"/>
       <c r="I45" s="15"/>
@@ -2259,15 +2198,15 @@
       <c r="AB45" s="14"/>
       <c r="AC45" s="15"/>
       <c r="AD45" s="16"/>
-      <c r="AE45"/>
-    </row>
-    <row r="46" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="26"/>
+      <c r="AE45" s="6"/>
+    </row>
+    <row r="46" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="12"/>
       <c r="G46" s="13"/>
       <c r="H46" s="14"/>
       <c r="I46" s="15"/>
@@ -2292,15 +2231,15 @@
       <c r="AB46" s="14"/>
       <c r="AC46" s="15"/>
       <c r="AD46" s="16"/>
-      <c r="AE46"/>
-    </row>
-    <row r="47" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="26"/>
+      <c r="AE46" s="6"/>
+    </row>
+    <row r="47" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="12"/>
       <c r="G47" s="13"/>
       <c r="H47" s="14"/>
       <c r="I47" s="15"/>
@@ -2325,15 +2264,15 @@
       <c r="AB47" s="14"/>
       <c r="AC47" s="15"/>
       <c r="AD47" s="16"/>
-      <c r="AE47"/>
-    </row>
-    <row r="48" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="26"/>
+      <c r="AE47" s="6"/>
+    </row>
+    <row r="48" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="12"/>
       <c r="G48" s="13"/>
       <c r="H48" s="14"/>
       <c r="I48" s="15"/>
@@ -2358,15 +2297,15 @@
       <c r="AB48" s="14"/>
       <c r="AC48" s="15"/>
       <c r="AD48" s="16"/>
-      <c r="AE48"/>
-    </row>
-    <row r="49" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="26"/>
+      <c r="AE48" s="6"/>
+    </row>
+    <row r="49" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="12"/>
       <c r="G49" s="13"/>
       <c r="H49" s="14"/>
       <c r="I49" s="15"/>
@@ -2391,15 +2330,15 @@
       <c r="AB49" s="14"/>
       <c r="AC49" s="15"/>
       <c r="AD49" s="16"/>
-      <c r="AE49"/>
-    </row>
-    <row r="50" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="26"/>
+      <c r="AE49" s="6"/>
+    </row>
+    <row r="50" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="12"/>
       <c r="G50" s="13"/>
       <c r="H50" s="14"/>
       <c r="I50" s="15"/>
@@ -2424,15 +2363,15 @@
       <c r="AB50" s="14"/>
       <c r="AC50" s="15"/>
       <c r="AD50" s="16"/>
-      <c r="AE50"/>
-    </row>
-    <row r="51" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="26"/>
+      <c r="AE50" s="6"/>
+    </row>
+    <row r="51" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="12"/>
       <c r="G51" s="13"/>
       <c r="H51" s="14"/>
       <c r="I51" s="15"/>
@@ -2457,15 +2396,15 @@
       <c r="AB51" s="14"/>
       <c r="AC51" s="15"/>
       <c r="AD51" s="16"/>
-      <c r="AE51"/>
-    </row>
-    <row r="52" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="25"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="26"/>
+      <c r="AE51" s="6"/>
+    </row>
+    <row r="52" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="12"/>
       <c r="G52" s="13"/>
       <c r="H52" s="14"/>
       <c r="I52" s="15"/>
@@ -2490,15 +2429,15 @@
       <c r="AB52" s="14"/>
       <c r="AC52" s="15"/>
       <c r="AD52" s="16"/>
-      <c r="AE52"/>
-    </row>
-    <row r="53" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="25"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="26"/>
+      <c r="AE52" s="6"/>
+    </row>
+    <row r="53" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="12"/>
       <c r="G53" s="13"/>
       <c r="H53" s="14"/>
       <c r="I53" s="15"/>
@@ -2523,15 +2462,15 @@
       <c r="AB53" s="14"/>
       <c r="AC53" s="15"/>
       <c r="AD53" s="16"/>
-      <c r="AE53"/>
-    </row>
-    <row r="54" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="26"/>
+      <c r="AE53" s="6"/>
+    </row>
+    <row r="54" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="12"/>
       <c r="G54" s="13"/>
       <c r="H54" s="14"/>
       <c r="I54" s="15"/>
@@ -2556,15 +2495,15 @@
       <c r="AB54" s="14"/>
       <c r="AC54" s="15"/>
       <c r="AD54" s="16"/>
-      <c r="AE54"/>
-    </row>
-    <row r="55" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="25"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="26"/>
+      <c r="AE54" s="6"/>
+    </row>
+    <row r="55" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="12"/>
       <c r="G55" s="13"/>
       <c r="H55" s="14"/>
       <c r="I55" s="15"/>
@@ -2589,15 +2528,15 @@
       <c r="AB55" s="14"/>
       <c r="AC55" s="15"/>
       <c r="AD55" s="16"/>
-      <c r="AE55"/>
-    </row>
-    <row r="56" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="25"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="26"/>
+      <c r="AE55" s="6"/>
+    </row>
+    <row r="56" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="12"/>
       <c r="G56" s="13"/>
       <c r="H56" s="14"/>
       <c r="I56" s="15"/>
@@ -2622,15 +2561,15 @@
       <c r="AB56" s="14"/>
       <c r="AC56" s="15"/>
       <c r="AD56" s="16"/>
-      <c r="AE56"/>
-    </row>
-    <row r="57" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="25"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="26"/>
+      <c r="AE56" s="6"/>
+    </row>
+    <row r="57" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="12"/>
       <c r="G57" s="13"/>
       <c r="H57" s="14"/>
       <c r="I57" s="15"/>
@@ -2655,15 +2594,15 @@
       <c r="AB57" s="14"/>
       <c r="AC57" s="15"/>
       <c r="AD57" s="16"/>
-      <c r="AE57"/>
-    </row>
-    <row r="58" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="25"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="27"/>
-      <c r="F58" s="26"/>
+      <c r="AE57" s="6"/>
+    </row>
+    <row r="58" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="12"/>
       <c r="G58" s="13"/>
       <c r="H58" s="14"/>
       <c r="I58" s="15"/>
@@ -2688,15 +2627,15 @@
       <c r="AB58" s="14"/>
       <c r="AC58" s="15"/>
       <c r="AD58" s="16"/>
-      <c r="AE58"/>
-    </row>
-    <row r="59" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="25"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="26"/>
+      <c r="AE58" s="6"/>
+    </row>
+    <row r="59" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="12"/>
       <c r="G59" s="13"/>
       <c r="H59" s="14"/>
       <c r="I59" s="15"/>
@@ -2721,15 +2660,15 @@
       <c r="AB59" s="14"/>
       <c r="AC59" s="15"/>
       <c r="AD59" s="16"/>
-      <c r="AE59"/>
-    </row>
-    <row r="60" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="25"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="26"/>
+      <c r="AE59" s="6"/>
+    </row>
+    <row r="60" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="12"/>
       <c r="G60" s="13"/>
       <c r="H60" s="14"/>
       <c r="I60" s="15"/>
@@ -2754,15 +2693,15 @@
       <c r="AB60" s="14"/>
       <c r="AC60" s="15"/>
       <c r="AD60" s="16"/>
-      <c r="AE60"/>
-    </row>
-    <row r="61" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE60" s="6"/>
+    </row>
+    <row r="61" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A61" s="8"/>
       <c r="B61" s="8"/>
       <c r="C61" s="9"/>
       <c r="D61" s="10"/>
       <c r="E61" s="11"/>
-      <c r="F61" s="17"/>
+      <c r="F61" s="12"/>
       <c r="G61" s="13"/>
       <c r="H61" s="14"/>
       <c r="I61" s="15"/>
@@ -2787,14 +2726,15 @@
       <c r="AB61" s="14"/>
       <c r="AC61" s="15"/>
       <c r="AD61" s="16"/>
-    </row>
-    <row r="62" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="18"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="19"/>
+      <c r="AE61" s="6"/>
+    </row>
+    <row r="62" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="12"/>
       <c r="G62" s="13"/>
       <c r="H62" s="14"/>
       <c r="I62" s="15"/>
@@ -2819,14 +2759,15 @@
       <c r="AB62" s="14"/>
       <c r="AC62" s="15"/>
       <c r="AD62" s="16"/>
-    </row>
-    <row r="63" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE62" s="6"/>
+    </row>
+    <row r="63" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A63" s="8"/>
       <c r="B63" s="8"/>
       <c r="C63" s="9"/>
       <c r="D63" s="10"/>
       <c r="E63" s="11"/>
-      <c r="F63" s="17"/>
+      <c r="F63" s="12"/>
       <c r="G63" s="13"/>
       <c r="H63" s="14"/>
       <c r="I63" s="15"/>
@@ -2851,14 +2792,14 @@
       <c r="AB63" s="14"/>
       <c r="AC63" s="15"/>
       <c r="AD63" s="16"/>
-      <c r="AE63"/>
-    </row>
-    <row r="64" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="21"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="22"/>
-      <c r="D64" s="22"/>
-      <c r="E64" s="23"/>
+      <c r="AE63" s="6"/>
+    </row>
+    <row r="64" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="11"/>
       <c r="F64" s="12"/>
       <c r="G64" s="13"/>
       <c r="H64" s="14"/>
@@ -2884,14 +2825,15 @@
       <c r="AB64" s="14"/>
       <c r="AC64" s="15"/>
       <c r="AD64" s="16"/>
-    </row>
-    <row r="65" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE64" s="6"/>
+    </row>
+    <row r="65" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
-      <c r="C65" s="10"/>
+      <c r="C65" s="9"/>
       <c r="D65" s="10"/>
       <c r="E65" s="11"/>
-      <c r="F65" s="28"/>
+      <c r="F65" s="12"/>
       <c r="G65" s="13"/>
       <c r="H65" s="14"/>
       <c r="I65" s="15"/>
@@ -2916,14 +2858,15 @@
       <c r="AB65" s="14"/>
       <c r="AC65" s="15"/>
       <c r="AD65" s="16"/>
-    </row>
-    <row r="66" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE65" s="6"/>
+    </row>
+    <row r="66" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A66" s="8"/>
       <c r="B66" s="8"/>
-      <c r="C66" s="10"/>
+      <c r="C66" s="9"/>
       <c r="D66" s="10"/>
       <c r="E66" s="11"/>
-      <c r="F66" s="28"/>
+      <c r="F66" s="12"/>
       <c r="G66" s="13"/>
       <c r="H66" s="14"/>
       <c r="I66" s="15"/>
@@ -2948,14 +2891,15 @@
       <c r="AB66" s="14"/>
       <c r="AC66" s="15"/>
       <c r="AD66" s="16"/>
-    </row>
-    <row r="67" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE66" s="6"/>
+    </row>
+    <row r="67" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="9"/>
       <c r="D67" s="10"/>
       <c r="E67" s="11"/>
-      <c r="F67" s="17"/>
+      <c r="F67" s="12"/>
       <c r="G67" s="13"/>
       <c r="H67" s="14"/>
       <c r="I67" s="15"/>
@@ -2980,14 +2924,15 @@
       <c r="AB67" s="14"/>
       <c r="AC67" s="15"/>
       <c r="AD67" s="16"/>
-    </row>
-    <row r="68" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="19"/>
+      <c r="AE67" s="6"/>
+    </row>
+    <row r="68" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="12"/>
       <c r="G68" s="13"/>
       <c r="H68" s="14"/>
       <c r="I68" s="15"/>
@@ -3012,14 +2957,15 @@
       <c r="AB68" s="14"/>
       <c r="AC68" s="15"/>
       <c r="AD68" s="16"/>
-    </row>
-    <row r="69" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A69" s="18"/>
-      <c r="B69" s="18"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="29"/>
+      <c r="AE68" s="6"/>
+    </row>
+    <row r="69" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A69" s="8"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="12"/>
       <c r="G69" s="13"/>
       <c r="H69" s="14"/>
       <c r="I69" s="15"/>
@@ -3044,13 +2990,14 @@
       <c r="AB69" s="14"/>
       <c r="AC69" s="15"/>
       <c r="AD69" s="16"/>
-    </row>
-    <row r="70" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A70" s="21"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="22"/>
-      <c r="D70" s="22"/>
-      <c r="E70" s="24"/>
+      <c r="AE69" s="6"/>
+    </row>
+    <row r="70" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="11"/>
       <c r="F70" s="12"/>
       <c r="G70" s="13"/>
       <c r="H70" s="14"/>
@@ -3076,14 +3023,15 @@
       <c r="AB70" s="14"/>
       <c r="AC70" s="15"/>
       <c r="AD70" s="16"/>
-    </row>
-    <row r="71" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AE70" s="6"/>
+    </row>
+    <row r="71" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A71" s="8"/>
       <c r="B71" s="8"/>
       <c r="C71" s="9"/>
       <c r="D71" s="10"/>
       <c r="E71" s="11"/>
-      <c r="F71" s="17"/>
+      <c r="F71" s="12"/>
       <c r="G71" s="13"/>
       <c r="H71" s="14"/>
       <c r="I71" s="15"/>
@@ -3108,14 +3056,15 @@
       <c r="AB71" s="14"/>
       <c r="AC71" s="15"/>
       <c r="AD71" s="16"/>
-    </row>
-    <row r="72" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A72" s="21"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="22"/>
-      <c r="D72" s="22"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="22"/>
+      <c r="AE71" s="6"/>
+    </row>
+    <row r="72" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="12"/>
       <c r="G72" s="13"/>
       <c r="H72" s="14"/>
       <c r="I72" s="15"/>
@@ -3140,14 +3089,15 @@
       <c r="AB72" s="14"/>
       <c r="AC72" s="15"/>
       <c r="AD72" s="16"/>
-    </row>
-    <row r="73" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A73" s="18"/>
-      <c r="B73" s="18"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="19"/>
+      <c r="AE72" s="6"/>
+    </row>
+    <row r="73" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A73" s="8"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="12"/>
       <c r="G73" s="13"/>
       <c r="H73" s="14"/>
       <c r="I73" s="15"/>
@@ -3172,14 +3122,15 @@
       <c r="AB73" s="14"/>
       <c r="AC73" s="15"/>
       <c r="AD73" s="16"/>
-    </row>
-    <row r="74" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A74" s="21"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="22"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="22"/>
+      <c r="AE73" s="6"/>
+    </row>
+    <row r="74" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="12"/>
       <c r="G74" s="13"/>
       <c r="H74" s="14"/>
       <c r="I74" s="15"/>
@@ -3204,14 +3155,15 @@
       <c r="AB74" s="14"/>
       <c r="AC74" s="15"/>
       <c r="AD74" s="16"/>
-    </row>
-    <row r="75" spans="1:31" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A75" s="18"/>
-      <c r="B75" s="18"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="19"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="19"/>
+      <c r="AE74" s="6"/>
+    </row>
+    <row r="75" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A75" s="8"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="12"/>
       <c r="G75" s="13"/>
       <c r="H75" s="14"/>
       <c r="I75" s="15"/>
@@ -3236,14 +3188,15 @@
       <c r="AB75" s="14"/>
       <c r="AC75" s="15"/>
       <c r="AD75" s="16"/>
-    </row>
-    <row r="76" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A76" s="21"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="22"/>
-      <c r="D76" s="22"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="22"/>
+      <c r="AE75" s="6"/>
+    </row>
+    <row r="76" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="12"/>
       <c r="G76" s="13"/>
       <c r="H76" s="14"/>
       <c r="I76" s="15"/>
@@ -3268,15 +3221,15 @@
       <c r="AB76" s="14"/>
       <c r="AC76" s="15"/>
       <c r="AD76" s="16"/>
-      <c r="AE76"/>
-    </row>
-    <row r="77" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A77" s="18"/>
-      <c r="B77" s="18"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="19"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="19"/>
+      <c r="AE76" s="6"/>
+    </row>
+    <row r="77" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="12"/>
       <c r="G77" s="13"/>
       <c r="H77" s="14"/>
       <c r="I77" s="15"/>
@@ -3301,15 +3254,15 @@
       <c r="AB77" s="14"/>
       <c r="AC77" s="15"/>
       <c r="AD77" s="16"/>
-      <c r="AE77"/>
-    </row>
-    <row r="78" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A78" s="21"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="22"/>
-      <c r="D78" s="22"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="22"/>
+      <c r="AE77" s="6"/>
+    </row>
+    <row r="78" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="12"/>
       <c r="G78" s="13"/>
       <c r="H78" s="14"/>
       <c r="I78" s="15"/>
@@ -3334,15 +3287,15 @@
       <c r="AB78" s="14"/>
       <c r="AC78" s="15"/>
       <c r="AD78" s="16"/>
-      <c r="AE78"/>
-    </row>
-    <row r="79" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A79" s="18"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="19"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="19"/>
+      <c r="AE78" s="6"/>
+    </row>
+    <row r="79" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="12"/>
       <c r="G79" s="13"/>
       <c r="H79" s="14"/>
       <c r="I79" s="15"/>
@@ -3367,15 +3320,15 @@
       <c r="AB79" s="14"/>
       <c r="AC79" s="15"/>
       <c r="AD79" s="16"/>
-      <c r="AE79"/>
-    </row>
-    <row r="80" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A80" s="21"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="22"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="22"/>
+      <c r="AE79" s="6"/>
+    </row>
+    <row r="80" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="12"/>
       <c r="G80" s="13"/>
       <c r="H80" s="14"/>
       <c r="I80" s="15"/>
@@ -3400,15 +3353,15 @@
       <c r="AB80" s="14"/>
       <c r="AC80" s="15"/>
       <c r="AD80" s="16"/>
-      <c r="AE80"/>
-    </row>
-    <row r="81" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A81" s="21"/>
-      <c r="B81" s="21"/>
-      <c r="C81" s="22"/>
-      <c r="D81" s="22"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="22"/>
+      <c r="AE80" s="6"/>
+    </row>
+    <row r="81" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A81" s="8"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="12"/>
       <c r="G81" s="13"/>
       <c r="H81" s="14"/>
       <c r="I81" s="15"/>
@@ -3433,15 +3386,15 @@
       <c r="AB81" s="14"/>
       <c r="AC81" s="15"/>
       <c r="AD81" s="16"/>
-      <c r="AE81"/>
-    </row>
-    <row r="82" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A82" s="18"/>
-      <c r="B82" s="18"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="19"/>
+      <c r="AE81" s="6"/>
+    </row>
+    <row r="82" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="12"/>
       <c r="G82" s="13"/>
       <c r="H82" s="14"/>
       <c r="I82" s="15"/>
@@ -3466,15 +3419,15 @@
       <c r="AB82" s="14"/>
       <c r="AC82" s="15"/>
       <c r="AD82" s="16"/>
-      <c r="AE82"/>
-    </row>
-    <row r="83" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A83" s="21"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="22"/>
-      <c r="D83" s="22"/>
-      <c r="E83" s="24"/>
-      <c r="F83" s="22"/>
+      <c r="AE82" s="6"/>
+    </row>
+    <row r="83" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A83" s="8"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="12"/>
       <c r="G83" s="13"/>
       <c r="H83" s="14"/>
       <c r="I83" s="15"/>
@@ -3499,15 +3452,15 @@
       <c r="AB83" s="14"/>
       <c r="AC83" s="15"/>
       <c r="AD83" s="16"/>
-      <c r="AE83"/>
-    </row>
-    <row r="84" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A84" s="18"/>
-      <c r="B84" s="18"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="19"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="19"/>
+      <c r="AE83" s="6"/>
+    </row>
+    <row r="84" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="12"/>
       <c r="G84" s="13"/>
       <c r="H84" s="14"/>
       <c r="I84" s="15"/>
@@ -3532,15 +3485,15 @@
       <c r="AB84" s="14"/>
       <c r="AC84" s="15"/>
       <c r="AD84" s="16"/>
-      <c r="AE84"/>
-    </row>
-    <row r="85" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A85" s="21"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="22"/>
+      <c r="AE84" s="6"/>
+    </row>
+    <row r="85" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A85" s="8"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="12"/>
       <c r="G85" s="13"/>
       <c r="H85" s="14"/>
       <c r="I85" s="15"/>
@@ -3565,15 +3518,15 @@
       <c r="AB85" s="14"/>
       <c r="AC85" s="15"/>
       <c r="AD85" s="16"/>
-      <c r="AE85"/>
-    </row>
-    <row r="86" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A86" s="18"/>
-      <c r="B86" s="18"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="19"/>
-      <c r="E86" s="20"/>
-      <c r="F86" s="19"/>
+      <c r="AE85" s="6"/>
+    </row>
+    <row r="86" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A86" s="8"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="12"/>
       <c r="G86" s="13"/>
       <c r="H86" s="14"/>
       <c r="I86" s="15"/>
@@ -3598,15 +3551,15 @@
       <c r="AB86" s="14"/>
       <c r="AC86" s="15"/>
       <c r="AD86" s="16"/>
-      <c r="AE86"/>
-    </row>
-    <row r="87" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A87" s="21"/>
-      <c r="B87" s="21"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="22"/>
+      <c r="AE86" s="6"/>
+    </row>
+    <row r="87" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="11"/>
+      <c r="F87" s="12"/>
       <c r="G87" s="13"/>
       <c r="H87" s="14"/>
       <c r="I87" s="15"/>
@@ -3631,15 +3584,15 @@
       <c r="AB87" s="14"/>
       <c r="AC87" s="15"/>
       <c r="AD87" s="16"/>
-      <c r="AE87"/>
-    </row>
-    <row r="88" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A88" s="21"/>
-      <c r="B88" s="21"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="22"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="22"/>
+      <c r="AE87" s="6"/>
+    </row>
+    <row r="88" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="11"/>
+      <c r="F88" s="12"/>
       <c r="G88" s="13"/>
       <c r="H88" s="14"/>
       <c r="I88" s="15"/>
@@ -3664,15 +3617,15 @@
       <c r="AB88" s="14"/>
       <c r="AC88" s="15"/>
       <c r="AD88" s="16"/>
-      <c r="AE88"/>
-    </row>
-    <row r="89" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A89" s="21"/>
-      <c r="B89" s="21"/>
-      <c r="C89" s="22"/>
-      <c r="D89" s="22"/>
-      <c r="E89" s="24"/>
-      <c r="F89" s="22"/>
+      <c r="AE88" s="6"/>
+    </row>
+    <row r="89" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="12"/>
       <c r="G89" s="13"/>
       <c r="H89" s="14"/>
       <c r="I89" s="15"/>
@@ -3697,15 +3650,15 @@
       <c r="AB89" s="14"/>
       <c r="AC89" s="15"/>
       <c r="AD89" s="16"/>
-      <c r="AE89"/>
-    </row>
-    <row r="90" spans="1:31" s="2" customFormat="1" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A90" s="18"/>
-      <c r="B90" s="18"/>
-      <c r="C90" s="19"/>
-      <c r="D90" s="19"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="19"/>
+      <c r="AE89" s="6"/>
+    </row>
+    <row r="90" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A90" s="8"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="12"/>
       <c r="G90" s="13"/>
       <c r="H90" s="14"/>
       <c r="I90" s="15"/>
@@ -3730,15 +3683,15 @@
       <c r="AB90" s="14"/>
       <c r="AC90" s="15"/>
       <c r="AD90" s="16"/>
-      <c r="AE90"/>
-    </row>
-    <row r="91" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A91" s="30"/>
-      <c r="B91" s="30"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="30"/>
+      <c r="AE90" s="6"/>
+    </row>
+    <row r="91" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A91" s="8"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="12"/>
       <c r="G91" s="13"/>
       <c r="H91" s="14"/>
       <c r="I91" s="15"/>
@@ -3763,15 +3716,15 @@
       <c r="AB91" s="14"/>
       <c r="AC91" s="15"/>
       <c r="AD91" s="16"/>
-      <c r="AE91"/>
-    </row>
-    <row r="92" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A92" s="30"/>
-      <c r="B92" s="30"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="30"/>
-      <c r="E92" s="30"/>
-      <c r="F92" s="30"/>
+      <c r="AE91" s="6"/>
+    </row>
+    <row r="92" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A92" s="8"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="12"/>
       <c r="G92" s="13"/>
       <c r="H92" s="14"/>
       <c r="I92" s="15"/>
@@ -3796,15 +3749,15 @@
       <c r="AB92" s="14"/>
       <c r="AC92" s="15"/>
       <c r="AD92" s="16"/>
-      <c r="AE92"/>
-    </row>
-    <row r="93" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A93" s="30"/>
-      <c r="B93" s="30"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="30"/>
-      <c r="E93" s="30"/>
-      <c r="F93" s="30"/>
+      <c r="AE92" s="6"/>
+    </row>
+    <row r="93" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A93" s="8"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="12"/>
       <c r="G93" s="13"/>
       <c r="H93" s="14"/>
       <c r="I93" s="15"/>
@@ -3829,15 +3782,15 @@
       <c r="AB93" s="14"/>
       <c r="AC93" s="15"/>
       <c r="AD93" s="16"/>
-      <c r="AE93"/>
-    </row>
-    <row r="94" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A94" s="30"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="30"/>
-      <c r="F94" s="30"/>
+      <c r="AE93" s="6"/>
+    </row>
+    <row r="94" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A94" s="8"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="12"/>
       <c r="G94" s="13"/>
       <c r="H94" s="14"/>
       <c r="I94" s="15"/>
@@ -3862,15 +3815,15 @@
       <c r="AB94" s="14"/>
       <c r="AC94" s="15"/>
       <c r="AD94" s="16"/>
-      <c r="AE94"/>
-    </row>
-    <row r="95" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A95" s="30"/>
-      <c r="B95" s="30"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="30"/>
-      <c r="E95" s="30"/>
-      <c r="F95" s="30"/>
+      <c r="AE94" s="6"/>
+    </row>
+    <row r="95" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="12"/>
       <c r="G95" s="13"/>
       <c r="H95" s="14"/>
       <c r="I95" s="15"/>
@@ -3895,15 +3848,15 @@
       <c r="AB95" s="14"/>
       <c r="AC95" s="15"/>
       <c r="AD95" s="16"/>
-      <c r="AE95"/>
-    </row>
-    <row r="96" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A96" s="30"/>
-      <c r="B96" s="30"/>
-      <c r="C96" s="30"/>
-      <c r="D96" s="30"/>
-      <c r="E96" s="30"/>
-      <c r="F96" s="30"/>
+      <c r="AE95" s="6"/>
+    </row>
+    <row r="96" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A96" s="8"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="12"/>
       <c r="G96" s="13"/>
       <c r="H96" s="14"/>
       <c r="I96" s="15"/>
@@ -3928,15 +3881,15 @@
       <c r="AB96" s="14"/>
       <c r="AC96" s="15"/>
       <c r="AD96" s="16"/>
-      <c r="AE96"/>
-    </row>
-    <row r="97" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A97" s="30"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="30"/>
-      <c r="D97" s="30"/>
-      <c r="E97" s="30"/>
-      <c r="F97" s="30"/>
+      <c r="AE96" s="6"/>
+    </row>
+    <row r="97" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A97" s="8"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="12"/>
       <c r="G97" s="13"/>
       <c r="H97" s="14"/>
       <c r="I97" s="15"/>
@@ -3961,15 +3914,15 @@
       <c r="AB97" s="14"/>
       <c r="AC97" s="15"/>
       <c r="AD97" s="16"/>
-      <c r="AE97"/>
-    </row>
-    <row r="98" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A98" s="30"/>
-      <c r="B98" s="30"/>
-      <c r="C98" s="30"/>
-      <c r="D98" s="30"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="30"/>
+      <c r="AE97" s="6"/>
+    </row>
+    <row r="98" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A98" s="8"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="12"/>
       <c r="G98" s="13"/>
       <c r="H98" s="14"/>
       <c r="I98" s="15"/>
@@ -3994,15 +3947,15 @@
       <c r="AB98" s="14"/>
       <c r="AC98" s="15"/>
       <c r="AD98" s="16"/>
-      <c r="AE98"/>
-    </row>
-    <row r="99" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A99"/>
-      <c r="B99"/>
-      <c r="C99"/>
-      <c r="D99"/>
-      <c r="E99"/>
-      <c r="F99"/>
+      <c r="AE98" s="6"/>
+    </row>
+    <row r="99" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A99" s="8"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="12"/>
       <c r="G99" s="13"/>
       <c r="H99" s="14"/>
       <c r="I99" s="15"/>
@@ -4027,15 +3980,15 @@
       <c r="AB99" s="14"/>
       <c r="AC99" s="15"/>
       <c r="AD99" s="16"/>
-      <c r="AE99"/>
-    </row>
-    <row r="100" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A100"/>
-      <c r="B100"/>
-      <c r="C100"/>
-      <c r="D100"/>
-      <c r="E100"/>
-      <c r="F100"/>
+      <c r="AE99" s="6"/>
+    </row>
+    <row r="100" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="12"/>
       <c r="G100" s="13"/>
       <c r="H100" s="14"/>
       <c r="I100" s="15"/>
@@ -4060,15 +4013,15 @@
       <c r="AB100" s="14"/>
       <c r="AC100" s="15"/>
       <c r="AD100" s="16"/>
-      <c r="AE100"/>
-    </row>
-    <row r="101" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A101"/>
-      <c r="B101"/>
-      <c r="C101"/>
-      <c r="D101"/>
-      <c r="E101"/>
-      <c r="F101"/>
+      <c r="AE100" s="6"/>
+    </row>
+    <row r="101" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A101" s="8"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="12"/>
       <c r="G101" s="13"/>
       <c r="H101" s="14"/>
       <c r="I101" s="15"/>
@@ -4093,15 +4046,15 @@
       <c r="AB101" s="14"/>
       <c r="AC101" s="15"/>
       <c r="AD101" s="16"/>
-      <c r="AE101"/>
-    </row>
-    <row r="102" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A102"/>
-      <c r="B102"/>
-      <c r="C102"/>
-      <c r="D102"/>
-      <c r="E102"/>
-      <c r="F102"/>
+      <c r="AE101" s="6"/>
+    </row>
+    <row r="102" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A102" s="8"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="11"/>
+      <c r="F102" s="12"/>
       <c r="G102" s="13"/>
       <c r="H102" s="14"/>
       <c r="I102" s="15"/>
@@ -4126,15 +4079,15 @@
       <c r="AB102" s="14"/>
       <c r="AC102" s="15"/>
       <c r="AD102" s="16"/>
-      <c r="AE102"/>
-    </row>
-    <row r="103" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A103"/>
-      <c r="B103"/>
-      <c r="C103"/>
-      <c r="D103"/>
-      <c r="E103"/>
-      <c r="F103"/>
+      <c r="AE102" s="6"/>
+    </row>
+    <row r="103" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A103" s="8"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="11"/>
+      <c r="F103" s="12"/>
       <c r="G103" s="13"/>
       <c r="H103" s="14"/>
       <c r="I103" s="15"/>
@@ -4159,15 +4112,15 @@
       <c r="AB103" s="14"/>
       <c r="AC103" s="15"/>
       <c r="AD103" s="16"/>
-      <c r="AE103"/>
-    </row>
-    <row r="104" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A104"/>
-      <c r="B104"/>
-      <c r="C104"/>
-      <c r="D104"/>
-      <c r="E104"/>
-      <c r="F104"/>
+      <c r="AE103" s="6"/>
+    </row>
+    <row r="104" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A104" s="8"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="10"/>
+      <c r="E104" s="11"/>
+      <c r="F104" s="12"/>
       <c r="G104" s="13"/>
       <c r="H104" s="14"/>
       <c r="I104" s="15"/>
@@ -4192,15 +4145,15 @@
       <c r="AB104" s="14"/>
       <c r="AC104" s="15"/>
       <c r="AD104" s="16"/>
-      <c r="AE104"/>
-    </row>
-    <row r="105" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A105"/>
-      <c r="B105"/>
-      <c r="C105"/>
-      <c r="D105"/>
-      <c r="E105"/>
-      <c r="F105"/>
+      <c r="AE104" s="6"/>
+    </row>
+    <row r="105" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A105" s="8"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="11"/>
+      <c r="F105" s="12"/>
       <c r="G105" s="13"/>
       <c r="H105" s="14"/>
       <c r="I105" s="15"/>
@@ -4225,15 +4178,15 @@
       <c r="AB105" s="14"/>
       <c r="AC105" s="15"/>
       <c r="AD105" s="16"/>
-      <c r="AE105"/>
-    </row>
-    <row r="106" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A106"/>
-      <c r="B106"/>
-      <c r="C106"/>
-      <c r="D106"/>
-      <c r="E106"/>
-      <c r="F106"/>
+      <c r="AE105" s="6"/>
+    </row>
+    <row r="106" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A106" s="8"/>
+      <c r="B106" s="8"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="10"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="12"/>
       <c r="G106" s="13"/>
       <c r="H106" s="14"/>
       <c r="I106" s="15"/>
@@ -4258,15 +4211,15 @@
       <c r="AB106" s="14"/>
       <c r="AC106" s="15"/>
       <c r="AD106" s="16"/>
-      <c r="AE106"/>
-    </row>
-    <row r="107" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A107"/>
-      <c r="B107"/>
-      <c r="C107"/>
-      <c r="D107"/>
-      <c r="E107"/>
-      <c r="F107"/>
+      <c r="AE106" s="6"/>
+    </row>
+    <row r="107" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A107" s="8"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="12"/>
       <c r="G107" s="13"/>
       <c r="H107" s="14"/>
       <c r="I107" s="15"/>
@@ -4291,15 +4244,15 @@
       <c r="AB107" s="14"/>
       <c r="AC107" s="15"/>
       <c r="AD107" s="16"/>
-      <c r="AE107"/>
-    </row>
-    <row r="108" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A108"/>
-      <c r="B108"/>
-      <c r="C108"/>
-      <c r="D108"/>
-      <c r="E108"/>
-      <c r="F108"/>
+      <c r="AE107" s="6"/>
+    </row>
+    <row r="108" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A108" s="8"/>
+      <c r="B108" s="8"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="12"/>
       <c r="G108" s="13"/>
       <c r="H108" s="14"/>
       <c r="I108" s="15"/>
@@ -4324,15 +4277,15 @@
       <c r="AB108" s="14"/>
       <c r="AC108" s="15"/>
       <c r="AD108" s="16"/>
-      <c r="AE108"/>
-    </row>
-    <row r="109" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A109"/>
-      <c r="B109"/>
-      <c r="C109"/>
-      <c r="D109"/>
-      <c r="E109"/>
-      <c r="F109"/>
+      <c r="AE108" s="6"/>
+    </row>
+    <row r="109" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A109" s="8"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="10"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="12"/>
       <c r="G109" s="13"/>
       <c r="H109" s="14"/>
       <c r="I109" s="15"/>
@@ -4357,15 +4310,15 @@
       <c r="AB109" s="14"/>
       <c r="AC109" s="15"/>
       <c r="AD109" s="16"/>
-      <c r="AE109"/>
-    </row>
-    <row r="110" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A110"/>
-      <c r="B110"/>
-      <c r="C110"/>
-      <c r="D110"/>
-      <c r="E110"/>
-      <c r="F110"/>
+      <c r="AE109" s="6"/>
+    </row>
+    <row r="110" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="10"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="12"/>
       <c r="G110" s="13"/>
       <c r="H110" s="14"/>
       <c r="I110" s="15"/>
@@ -4390,15 +4343,15 @@
       <c r="AB110" s="14"/>
       <c r="AC110" s="15"/>
       <c r="AD110" s="16"/>
-      <c r="AE110"/>
-    </row>
-    <row r="111" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A111"/>
-      <c r="B111"/>
-      <c r="C111"/>
-      <c r="D111"/>
-      <c r="E111"/>
-      <c r="F111"/>
+      <c r="AE110" s="6"/>
+    </row>
+    <row r="111" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A111" s="8"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="11"/>
+      <c r="F111" s="12"/>
       <c r="G111" s="13"/>
       <c r="H111" s="14"/>
       <c r="I111" s="15"/>
@@ -4423,15 +4376,15 @@
       <c r="AB111" s="14"/>
       <c r="AC111" s="15"/>
       <c r="AD111" s="16"/>
-      <c r="AE111"/>
-    </row>
-    <row r="112" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A112"/>
-      <c r="B112"/>
-      <c r="C112"/>
-      <c r="D112"/>
-      <c r="E112"/>
-      <c r="F112"/>
+      <c r="AE111" s="6"/>
+    </row>
+    <row r="112" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="12"/>
       <c r="G112" s="13"/>
       <c r="H112" s="14"/>
       <c r="I112" s="15"/>
@@ -4456,15 +4409,15 @@
       <c r="AB112" s="14"/>
       <c r="AC112" s="15"/>
       <c r="AD112" s="16"/>
-      <c r="AE112"/>
-    </row>
-    <row r="113" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A113"/>
-      <c r="B113"/>
-      <c r="C113"/>
-      <c r="D113"/>
-      <c r="E113"/>
-      <c r="F113"/>
+      <c r="AE112" s="6"/>
+    </row>
+    <row r="113" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A113" s="8"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="10"/>
+      <c r="E113" s="11"/>
+      <c r="F113" s="12"/>
       <c r="G113" s="13"/>
       <c r="H113" s="14"/>
       <c r="I113" s="15"/>
@@ -4489,15 +4442,15 @@
       <c r="AB113" s="14"/>
       <c r="AC113" s="15"/>
       <c r="AD113" s="16"/>
-      <c r="AE113"/>
-    </row>
-    <row r="114" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A114"/>
-      <c r="B114"/>
-      <c r="C114"/>
-      <c r="D114"/>
-      <c r="E114"/>
-      <c r="F114"/>
+      <c r="AE113" s="6"/>
+    </row>
+    <row r="114" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A114" s="8"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="9"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="12"/>
       <c r="G114" s="13"/>
       <c r="H114" s="14"/>
       <c r="I114" s="15"/>
@@ -4522,15 +4475,15 @@
       <c r="AB114" s="14"/>
       <c r="AC114" s="15"/>
       <c r="AD114" s="16"/>
-      <c r="AE114"/>
-    </row>
-    <row r="115" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A115"/>
-      <c r="B115"/>
-      <c r="C115"/>
-      <c r="D115"/>
-      <c r="E115"/>
-      <c r="F115"/>
+      <c r="AE114" s="6"/>
+    </row>
+    <row r="115" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A115" s="8"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="9"/>
+      <c r="D115" s="10"/>
+      <c r="E115" s="11"/>
+      <c r="F115" s="12"/>
       <c r="G115" s="13"/>
       <c r="H115" s="14"/>
       <c r="I115" s="15"/>
@@ -4555,15 +4508,15 @@
       <c r="AB115" s="14"/>
       <c r="AC115" s="15"/>
       <c r="AD115" s="16"/>
-      <c r="AE115"/>
-    </row>
-    <row r="116" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A116"/>
-      <c r="B116"/>
-      <c r="C116"/>
-      <c r="D116"/>
-      <c r="E116"/>
-      <c r="F116"/>
+      <c r="AE115" s="6"/>
+    </row>
+    <row r="116" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A116" s="8"/>
+      <c r="B116" s="8"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="10"/>
+      <c r="E116" s="11"/>
+      <c r="F116" s="12"/>
       <c r="G116" s="13"/>
       <c r="H116" s="14"/>
       <c r="I116" s="15"/>
@@ -4588,15 +4541,15 @@
       <c r="AB116" s="14"/>
       <c r="AC116" s="15"/>
       <c r="AD116" s="16"/>
-      <c r="AE116"/>
-    </row>
-    <row r="117" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A117"/>
-      <c r="B117"/>
-      <c r="C117"/>
-      <c r="D117"/>
-      <c r="E117"/>
-      <c r="F117"/>
+      <c r="AE116" s="6"/>
+    </row>
+    <row r="117" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="11"/>
+      <c r="F117" s="12"/>
       <c r="G117" s="13"/>
       <c r="H117" s="14"/>
       <c r="I117" s="15"/>
@@ -4621,15 +4574,15 @@
       <c r="AB117" s="14"/>
       <c r="AC117" s="15"/>
       <c r="AD117" s="16"/>
-      <c r="AE117"/>
-    </row>
-    <row r="118" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A118"/>
-      <c r="B118"/>
-      <c r="C118"/>
-      <c r="D118"/>
-      <c r="E118"/>
-      <c r="F118"/>
+      <c r="AE117" s="6"/>
+    </row>
+    <row r="118" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="10"/>
+      <c r="E118" s="11"/>
+      <c r="F118" s="12"/>
       <c r="G118" s="13"/>
       <c r="H118" s="14"/>
       <c r="I118" s="15"/>
@@ -4654,15 +4607,15 @@
       <c r="AB118" s="14"/>
       <c r="AC118" s="15"/>
       <c r="AD118" s="16"/>
-      <c r="AE118"/>
-    </row>
-    <row r="119" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A119"/>
-      <c r="B119"/>
-      <c r="C119"/>
-      <c r="D119"/>
-      <c r="E119"/>
-      <c r="F119"/>
+      <c r="AE118" s="6"/>
+    </row>
+    <row r="119" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A119" s="8"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="11"/>
+      <c r="F119" s="12"/>
       <c r="G119" s="13"/>
       <c r="H119" s="14"/>
       <c r="I119" s="15"/>
@@ -4687,15 +4640,15 @@
       <c r="AB119" s="14"/>
       <c r="AC119" s="15"/>
       <c r="AD119" s="16"/>
-      <c r="AE119"/>
-    </row>
-    <row r="120" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A120"/>
-      <c r="B120"/>
-      <c r="C120"/>
-      <c r="D120"/>
-      <c r="E120"/>
-      <c r="F120"/>
+      <c r="AE119" s="6"/>
+    </row>
+    <row r="120" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="10"/>
+      <c r="E120" s="11"/>
+      <c r="F120" s="12"/>
       <c r="G120" s="13"/>
       <c r="H120" s="14"/>
       <c r="I120" s="15"/>
@@ -4720,15 +4673,15 @@
       <c r="AB120" s="14"/>
       <c r="AC120" s="15"/>
       <c r="AD120" s="16"/>
-      <c r="AE120"/>
-    </row>
-    <row r="121" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A121"/>
-      <c r="B121"/>
-      <c r="C121"/>
-      <c r="D121"/>
-      <c r="E121"/>
-      <c r="F121"/>
+      <c r="AE120" s="6"/>
+    </row>
+    <row r="121" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A121" s="8"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="10"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="12"/>
       <c r="G121" s="13"/>
       <c r="H121" s="14"/>
       <c r="I121" s="15"/>
@@ -4753,15 +4706,15 @@
       <c r="AB121" s="14"/>
       <c r="AC121" s="15"/>
       <c r="AD121" s="16"/>
-      <c r="AE121"/>
-    </row>
-    <row r="122" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A122"/>
-      <c r="B122"/>
-      <c r="C122"/>
-      <c r="D122"/>
-      <c r="E122"/>
-      <c r="F122"/>
+      <c r="AE121" s="6"/>
+    </row>
+    <row r="122" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="11"/>
+      <c r="F122" s="12"/>
       <c r="G122" s="13"/>
       <c r="H122" s="14"/>
       <c r="I122" s="15"/>
@@ -4786,15 +4739,15 @@
       <c r="AB122" s="14"/>
       <c r="AC122" s="15"/>
       <c r="AD122" s="16"/>
-      <c r="AE122"/>
-    </row>
-    <row r="123" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A123"/>
-      <c r="B123"/>
-      <c r="C123"/>
-      <c r="D123"/>
-      <c r="E123"/>
-      <c r="F123"/>
+      <c r="AE122" s="6"/>
+    </row>
+    <row r="123" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A123" s="8"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="11"/>
+      <c r="F123" s="12"/>
       <c r="G123" s="13"/>
       <c r="H123" s="14"/>
       <c r="I123" s="15"/>
@@ -4819,15 +4772,15 @@
       <c r="AB123" s="14"/>
       <c r="AC123" s="15"/>
       <c r="AD123" s="16"/>
-      <c r="AE123"/>
-    </row>
-    <row r="124" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A124"/>
-      <c r="B124"/>
-      <c r="C124"/>
-      <c r="D124"/>
-      <c r="E124"/>
-      <c r="F124"/>
+      <c r="AE123" s="6"/>
+    </row>
+    <row r="124" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A124" s="8"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="10"/>
+      <c r="E124" s="11"/>
+      <c r="F124" s="12"/>
       <c r="G124" s="13"/>
       <c r="H124" s="14"/>
       <c r="I124" s="15"/>
@@ -4852,15 +4805,15 @@
       <c r="AB124" s="14"/>
       <c r="AC124" s="15"/>
       <c r="AD124" s="16"/>
-      <c r="AE124"/>
-    </row>
-    <row r="125" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A125"/>
-      <c r="B125"/>
-      <c r="C125"/>
-      <c r="D125"/>
-      <c r="E125"/>
-      <c r="F125"/>
+      <c r="AE124" s="6"/>
+    </row>
+    <row r="125" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A125" s="8"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="9"/>
+      <c r="D125" s="10"/>
+      <c r="E125" s="11"/>
+      <c r="F125" s="12"/>
       <c r="G125" s="13"/>
       <c r="H125" s="14"/>
       <c r="I125" s="15"/>
@@ -4885,15 +4838,15 @@
       <c r="AB125" s="14"/>
       <c r="AC125" s="15"/>
       <c r="AD125" s="16"/>
-      <c r="AE125"/>
-    </row>
-    <row r="126" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A126"/>
-      <c r="B126"/>
-      <c r="C126"/>
-      <c r="D126"/>
-      <c r="E126"/>
-      <c r="F126"/>
+      <c r="AE125" s="6"/>
+    </row>
+    <row r="126" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A126" s="8"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="10"/>
+      <c r="E126" s="11"/>
+      <c r="F126" s="12"/>
       <c r="G126" s="13"/>
       <c r="H126" s="14"/>
       <c r="I126" s="15"/>
@@ -4918,15 +4871,15 @@
       <c r="AB126" s="14"/>
       <c r="AC126" s="15"/>
       <c r="AD126" s="16"/>
-      <c r="AE126"/>
-    </row>
-    <row r="127" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A127"/>
-      <c r="B127"/>
-      <c r="C127"/>
-      <c r="D127"/>
-      <c r="E127"/>
-      <c r="F127"/>
+      <c r="AE126" s="6"/>
+    </row>
+    <row r="127" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A127" s="8"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="11"/>
+      <c r="F127" s="12"/>
       <c r="G127" s="13"/>
       <c r="H127" s="14"/>
       <c r="I127" s="15"/>
@@ -4951,15 +4904,15 @@
       <c r="AB127" s="14"/>
       <c r="AC127" s="15"/>
       <c r="AD127" s="16"/>
-      <c r="AE127"/>
-    </row>
-    <row r="128" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A128"/>
-      <c r="B128"/>
-      <c r="C128"/>
-      <c r="D128"/>
-      <c r="E128"/>
-      <c r="F128"/>
+      <c r="AE127" s="6"/>
+    </row>
+    <row r="128" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A128" s="8"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="10"/>
+      <c r="E128" s="11"/>
+      <c r="F128" s="12"/>
       <c r="G128" s="13"/>
       <c r="H128" s="14"/>
       <c r="I128" s="15"/>
@@ -4984,15 +4937,15 @@
       <c r="AB128" s="14"/>
       <c r="AC128" s="15"/>
       <c r="AD128" s="16"/>
-      <c r="AE128"/>
-    </row>
-    <row r="129" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
-      <c r="A129"/>
-      <c r="B129"/>
-      <c r="C129"/>
-      <c r="D129"/>
-      <c r="E129"/>
-      <c r="F129"/>
+      <c r="AE128" s="6"/>
+    </row>
+    <row r="129" spans="1:31" ht="34.5" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="A129" s="8"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="10"/>
+      <c r="E129" s="11"/>
+      <c r="F129" s="12"/>
       <c r="G129" s="13"/>
       <c r="H129" s="14"/>
       <c r="I129" s="15"/>
@@ -5017,9 +4970,9 @@
       <c r="AB129" s="14"/>
       <c r="AC129" s="15"/>
       <c r="AD129" s="16"/>
-      <c r="AE129"/>
-    </row>
-    <row r="130" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+      <c r="AE129" s="6"/>
+    </row>
+    <row r="130" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A130"/>
       <c r="B130"/>
       <c r="C130"/>
@@ -5052,7 +5005,7 @@
       <c r="AD130" s="16"/>
       <c r="AE130"/>
     </row>
-    <row r="131" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A131"/>
       <c r="B131"/>
       <c r="C131"/>
@@ -5085,7 +5038,7 @@
       <c r="AD131" s="16"/>
       <c r="AE131"/>
     </row>
-    <row r="132" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A132"/>
       <c r="B132"/>
       <c r="C132"/>
@@ -5118,7 +5071,7 @@
       <c r="AD132" s="16"/>
       <c r="AE132"/>
     </row>
-    <row r="133" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A133"/>
       <c r="B133"/>
       <c r="C133"/>
@@ -5151,7 +5104,7 @@
       <c r="AD133" s="16"/>
       <c r="AE133"/>
     </row>
-    <row r="134" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A134"/>
       <c r="B134"/>
       <c r="C134"/>
@@ -5184,7 +5137,7 @@
       <c r="AD134" s="16"/>
       <c r="AE134"/>
     </row>
-    <row r="135" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A135"/>
       <c r="B135"/>
       <c r="C135"/>
@@ -5217,7 +5170,7 @@
       <c r="AD135" s="16"/>
       <c r="AE135"/>
     </row>
-    <row r="136" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A136"/>
       <c r="B136"/>
       <c r="C136"/>
@@ -5250,7 +5203,7 @@
       <c r="AD136" s="16"/>
       <c r="AE136"/>
     </row>
-    <row r="137" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A137"/>
       <c r="B137"/>
       <c r="C137"/>
@@ -5283,7 +5236,7 @@
       <c r="AD137" s="16"/>
       <c r="AE137"/>
     </row>
-    <row r="138" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A138"/>
       <c r="B138"/>
       <c r="C138"/>
@@ -5316,7 +5269,7 @@
       <c r="AD138" s="16"/>
       <c r="AE138"/>
     </row>
-    <row r="139" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A139"/>
       <c r="B139"/>
       <c r="C139"/>
@@ -5349,7 +5302,7 @@
       <c r="AD139" s="16"/>
       <c r="AE139"/>
     </row>
-    <row r="140" spans="1:31" s="2" customFormat="1" ht="33.75" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:31" s="2" customFormat="1" ht="33.6" x14ac:dyDescent="0.4">
       <c r="A140"/>
       <c r="B140"/>
       <c r="C140"/>

</xml_diff>